<commit_message>
Adicionando horas trabalhadas no relatorio
</commit_message>
<xml_diff>
--- a/Documentacao/GERENCIA/RelatorioDetalhadoAtividades.xlsx
+++ b/Documentacao/GERENCIA/RelatorioDetalhadoAtividades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t xml:space="preserve">Relatorio Detalhado de Atividades</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">Total de Horas</t>
   </si>
   <si>
+    <t xml:space="preserve">Relatório</t>
+  </si>
+  <si>
     <t xml:space="preserve">Especificação dos 5 casos de uso</t>
   </si>
   <si>
@@ -78,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cotação realizada por Faberson, foi realizada conferência e pequenas alterações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doa 08/10 finalização do documento, termino dos requisitos funcionais e não funcionais e sumário </t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]H:MM:SS\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="H:MM:SS\ AM/PM"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -393,9 +399,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208960</xdr:colOff>
+      <xdr:colOff>2208600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>360720</xdr:rowOff>
+      <xdr:rowOff>360360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -407,7 +413,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="1171440"/>
-          <a:ext cx="761040" cy="332280"/>
+          <a:ext cx="760680" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -465,9 +471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208960</xdr:colOff>
+      <xdr:colOff>2208600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>360720</xdr:rowOff>
+      <xdr:rowOff>360360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -479,7 +485,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="1933200"/>
-          <a:ext cx="761040" cy="332280"/>
+          <a:ext cx="760680" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -537,9 +543,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208960</xdr:colOff>
+      <xdr:colOff>2208600</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>360720</xdr:rowOff>
+      <xdr:rowOff>360360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -551,7 +557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="2314440"/>
-          <a:ext cx="761040" cy="332280"/>
+          <a:ext cx="760680" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -609,9 +615,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208960</xdr:colOff>
+      <xdr:colOff>2208600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>360720</xdr:rowOff>
+      <xdr:rowOff>360360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -623,7 +629,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="1552320"/>
-          <a:ext cx="761040" cy="332280"/>
+          <a:ext cx="760680" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -681,9 +687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1323000</xdr:colOff>
+      <xdr:colOff>1322640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -697,7 +703,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="66600"/>
-          <a:ext cx="1323000" cy="322560"/>
+          <a:ext cx="1322640" cy="322200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -744,11 +750,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela818" displayName="Tabela818" ref="A1:C6" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
-  <autoFilter ref="A1:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela818" displayName="Tabela818" ref="A1:C7" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
+  <autoFilter ref="A1:C7"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Atividade"/>
-    <tableColumn id="2" name="Relatorio"/>
+    <tableColumn id="2" name="Relatório"/>
     <tableColumn id="3" name="Horas"/>
   </tableColumns>
 </table>
@@ -830,7 +836,7 @@
       </c>
       <c r="B6" s="6" t="n">
         <f aca="false">Tabela818[[#Totals],[Horas]]</f>
-        <v>0.635416666666666</v>
+        <v>0.781249999999999</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -942,10 +948,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C138"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -956,12 +962,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>2</v>
@@ -969,10 +975,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>0.208333333333333</v>
@@ -980,10 +986,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>0.25</v>
@@ -991,10 +997,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>0.145833333333333</v>
@@ -1002,25 +1008,39 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>0.03125</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="12" t="n">
+        <v>0.145833333333333</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="n">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="n">
         <f aca="false">SUM(Tabela818[Horas])</f>
-        <v>0.635416666666666</v>
-      </c>
-    </row>
+        <v>0.781249999999999</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Atualização no cronograma e no relatorio detalhado de atividades
</commit_message>
<xml_diff>
--- a/Documentacao/GERENCIA/RelatorioDetalhadoAtividades.xlsx
+++ b/Documentacao/GERENCIA/RelatorioDetalhadoAtividades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,12 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">Relatorio Detalhado de Atividades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relatori de Atividades</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">Relatório Detalhado de Atividades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colaboradores</t>
   </si>
   <si>
     <t xml:space="preserve">Horas</t>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">Faberson</t>
   </si>
   <si>
-    <t xml:space="preserve">Felipe</t>
+    <t xml:space="preserve">Felipe (Gerente)</t>
   </si>
   <si>
     <t xml:space="preserve">Marcelo</t>
@@ -83,7 +83,13 @@
     <t xml:space="preserve">Cotação realizada por Faberson, foi realizada conferência e pequenas alterações</t>
   </si>
   <si>
-    <t xml:space="preserve">Doa 08/10 finalização do documento, termino dos requisitos funcionais e não funcionais e sumário </t>
+    <t xml:space="preserve">Dia 08/10 finalização do documento, termino dos requisitos funcionais e não funcionais e sumário </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustes finais para a 2° entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustes finais nos documentos para 2° entrega</t>
   </si>
 </sst>
 </file>
@@ -399,9 +405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208600</xdr:colOff>
+      <xdr:colOff>2208240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>360360</xdr:rowOff>
+      <xdr:rowOff>360000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -413,7 +419,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="1171440"/>
-          <a:ext cx="760680" cy="331920"/>
+          <a:ext cx="760320" cy="331560"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -471,9 +477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208600</xdr:colOff>
+      <xdr:colOff>2208240</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>360360</xdr:rowOff>
+      <xdr:rowOff>360000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -485,7 +491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="1933200"/>
-          <a:ext cx="760680" cy="331920"/>
+          <a:ext cx="760320" cy="331560"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -543,9 +549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208600</xdr:colOff>
+      <xdr:colOff>2208240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>360360</xdr:rowOff>
+      <xdr:rowOff>360000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -557,7 +563,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="2314440"/>
-          <a:ext cx="760680" cy="331920"/>
+          <a:ext cx="760320" cy="331560"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -615,9 +621,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2208600</xdr:colOff>
+      <xdr:colOff>2208240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>360360</xdr:rowOff>
+      <xdr:rowOff>360000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -629,7 +635,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1447920" y="1552320"/>
-          <a:ext cx="760680" cy="331920"/>
+          <a:ext cx="760320" cy="331560"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -687,9 +693,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1322640</xdr:colOff>
+      <xdr:colOff>1322280</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -703,7 +709,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="66600"/>
-          <a:ext cx="1322640" cy="322200"/>
+          <a:ext cx="1322280" cy="321840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -721,7 +727,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela7" displayName="Tabela7" ref="A3:B7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Relatori de Atividades"/>
+    <tableColumn id="1" name="Colaboradores"/>
     <tableColumn id="2" name="Horas"/>
   </tableColumns>
 </table>
@@ -750,8 +756,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela818" displayName="Tabela818" ref="A1:C7" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
-  <autoFilter ref="A1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela818" displayName="Tabela818" ref="A1:C8" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Atividade"/>
     <tableColumn id="2" name="Relatório"/>
@@ -778,8 +784,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -836,7 +842,7 @@
       </c>
       <c r="B6" s="6" t="n">
         <f aca="false">Tabela818[[#Totals],[Horas]]</f>
-        <v>0.781249999999999</v>
+        <v>0.802083333333333</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -948,10 +954,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1028,19 +1034,30 @@
         <v>0.145833333333333</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="12" t="n">
+        <v>0.0208333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="n">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15" t="n">
         <f aca="false">SUM(Tabela818[Horas])</f>
-        <v>0.781249999999999</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>0.802083333333333</v>
+      </c>
+    </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>